<commit_message>
modifying LLP Jet seed
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v0_1_5/PrescaleTable/L1Menu_Collisions2022_v0_1_5.xlsx
+++ b/development/L1Menu_Collisions2022_v0_1_5/PrescaleTable/L1Menu_Collisions2022_v0_1_5.xlsx
@@ -118,7 +118,7 @@
     <t>L1_SingleMu25</t>
   </si>
   <si>
-    <t>L1_SingleJet35_llp</t>
+    <t>L1_HTT120_SingleLLPJet40</t>
   </si>
   <si>
     <t>L1_SingleMu6er1p5</t>
@@ -1305,16 +1305,16 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1486,9 +1486,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1568,7 +1568,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1596,10 +1596,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1855,9 +1855,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -2145,7 +2145,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2173,10 +2173,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2434,7 +2434,7 @@
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.9844" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27" style="1" customWidth="1"/>
     <col min="3" max="11" width="8.85156" style="1" customWidth="1"/>
     <col min="12" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>

</xml_diff>